<commit_message>
fake or real news
</commit_message>
<xml_diff>
--- a/test_data/Data.xlsx
+++ b/test_data/Data.xlsx
@@ -1260,7 +1260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,7 +1522,139 @@
           <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Outlook India, The Hans India, Deccan Herald</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>tungabhadra dam gate crash</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>18 Aug 2024</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Outlook India, Deccan Herald, The Hans India</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>double decker flyover in bengaluru</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>26 Jul 2024</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>The double-decker flyover features two separate carriageways, each with two lanes. It passes by three metro stations: Jayadeva Hospital,...</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>The Hindu, NDTV, Hindustan Times, Times of India</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>tungabhadra dam crash</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>18 Aug 2024</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Outlook India, The Hans India, Deccan Herald</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>Tungabhadra Dam crash</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>18 Aug 2024</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>The Hans India, Deccan Herald, Outlook India</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>tungabhadra dam gate crash</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>16 Aug 2024</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>Outlook India, The Hans India, Deccan Herald</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>tungabhadra dam crash</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>16 Aug 2024</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>Several attempts to fix the breach in crest gate number 19 of Tungabhadra dam failed to yield the desired results on Thursday. ADVERTISEMENT.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>Outlook India, The Hans India, Deccan Herald</t>
         </is>

</xml_diff>